<commit_message>
[FIX] 【upgrade to 0.1.1】 fix uncorrent content2list(parts of), fix lastest menu and init excel
</commit_message>
<xml_diff>
--- a/src/main/resources/script/front/micro-service-init-data.xlsx
+++ b/src/main/resources/script/front/micro-service-init-data.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>/iam/send-setting</t>
+          <t>/notify/send-setting</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>/iam/mail-template</t>
+          <t>/notify/mail-template</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>/iam/inmail-template</t>
+          <t>/notify/inmail-template</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>/iam/mail-setting</t>
+          <t>/notify/mail-setting</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>/iam/msg-record</t>
+          <t>/notify/msg-record</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>/iam/announcement</t>
+          <t>/notify/announcement</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>/iam/user-msg</t>
+          <t>/notify/user-msg</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>/iam/receive-setting</t>
+          <t>/notify/receive-setting</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">

</xml_diff>